<commit_message>
Añadida visualización de rango central en ablación
</commit_message>
<xml_diff>
--- a/models/ATT2ITM/pois/madrid/afe7526023b1827d88ecad6479de8971/att_text.xlsx
+++ b/models/ATT2ITM/pois/madrid/afe7526023b1827d88ecad6479de8971/att_text.xlsx
@@ -421,7 +421,7 @@
     <t>Wanda Metropolitano</t>
   </si>
   <si>
-    <t>no</t>
+    <t>el</t>
   </si>
 </sst>
 </file>
@@ -803,7 +803,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-0.001722647459246218</v>
+        <v>-0.01418817136436701</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -811,7 +811,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.01927484013140202</v>
+        <v>-0.01503446325659752</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -819,7 +819,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.07653801888227463</v>
+        <v>0.03324057534337044</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -827,7 +827,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.04841911420226097</v>
+        <v>0.02983036078512669</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -835,7 +835,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.04836303368210793</v>
+        <v>0.0356731005012989</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -843,7 +843,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.1410248726606369</v>
+        <v>-0.038100965321064</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -851,7 +851,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-0.002377573866397142</v>
+        <v>0.03669719398021698</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -859,7 +859,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.03937764093279839</v>
+        <v>0.03898508101701736</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -867,7 +867,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-0.09736644476652145</v>
+        <v>-0.06035224720835686</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -875,7 +875,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-0.07721391320228577</v>
+        <v>-0.02828722260892391</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -883,7 +883,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-0.06910920143127441</v>
+        <v>-0.01741178147494793</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -891,7 +891,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.007316585630178452</v>
+        <v>0.02714044786989689</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -899,7 +899,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0.01572574861347675</v>
+        <v>0.008196081034839153</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -907,7 +907,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-0.2201144099235535</v>
+        <v>0.02671819180250168</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -915,7 +915,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.0306585468351841</v>
+        <v>0.004293262492865324</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -923,7 +923,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>-0.1006064489483833</v>
+        <v>-0.0127369137480855</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -931,7 +931,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>-0.007895681075751781</v>
+        <v>-0.08475329726934433</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -939,7 +939,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>-0.10365080088377</v>
+        <v>-0.05107626691460609</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -947,7 +947,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>-0.06342870742082596</v>
+        <v>-0.01093430444598198</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -955,7 +955,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>-0.1475490182638168</v>
+        <v>0.01788171194493771</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -963,7 +963,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>0.0628189891576767</v>
+        <v>0.0005421822424978018</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -971,7 +971,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0.05929253995418549</v>
+        <v>-0.06557711213827133</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -979,7 +979,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>-0.01987669989466667</v>
+        <v>0.01326756551861763</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -987,7 +987,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>-0.05435210093855858</v>
+        <v>0.01878784783184528</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -995,7 +995,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>-0.03779342770576477</v>
+        <v>-0.02680497989058495</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1003,7 +1003,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>-0.02487851120531559</v>
+        <v>-0.03166486695408821</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1011,7 +1011,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>-0.003557308111339808</v>
+        <v>0.05254664272069931</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1019,7 +1019,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0.06167079880833626</v>
+        <v>-0.004024737048894167</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1027,7 +1027,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>-0.04274114966392517</v>
+        <v>-0.03146779537200928</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1035,7 +1035,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>-0.03368065133690834</v>
+        <v>0.04504603520035744</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1043,7 +1043,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>-0.1755696684122086</v>
+        <v>0.05009873956441879</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1051,7 +1051,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>-0.1354453861713409</v>
+        <v>-0.06726761162281036</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1059,7 +1059,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>-0.06961099803447723</v>
+        <v>-0.0009220695937983692</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1067,7 +1067,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>-0.06197665259242058</v>
+        <v>0.004506095312535763</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1075,7 +1075,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>-0.07049228996038437</v>
+        <v>-0.02105730772018433</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1083,7 +1083,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>-0.01084873173385859</v>
+        <v>0.001260937424376607</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1091,7 +1091,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>-0.1619250625371933</v>
+        <v>-0.03853989392518997</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1099,7 +1099,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0.01109087653458118</v>
+        <v>0.0006460323347710073</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1107,7 +1107,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>-0.01711871288716793</v>
+        <v>-0.01117102708667517</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1115,7 +1115,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>-0.06481350213289261</v>
+        <v>0.05321109294891357</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1123,7 +1123,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>0.04046884924173355</v>
+        <v>0.02866742201149464</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1131,7 +1131,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>-0.1680614650249481</v>
+        <v>-0.1117166131734848</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1139,7 +1139,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>-0.1273567825555801</v>
+        <v>-0.04144596308469772</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1147,7 +1147,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>0.04559533670544624</v>
+        <v>0.03518811240792274</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1155,7 +1155,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>-0.07777110487222672</v>
+        <v>0.01006702240556479</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1163,7 +1163,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>-0.07063893228769302</v>
+        <v>-0.006136109586805105</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1171,7 +1171,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>-0.07966483384370804</v>
+        <v>-0.02939275465905666</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1179,7 +1179,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>-0.0713554248213768</v>
+        <v>-0.01789583824574947</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1187,7 +1187,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>-0.1464598178863525</v>
+        <v>-0.005569220054894686</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1195,7 +1195,7 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>-0.06632831692695618</v>
+        <v>-0.06661555916070938</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1203,7 +1203,7 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0.008580437861382961</v>
+        <v>-0.02575983107089996</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1211,7 +1211,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>0.05825182050466537</v>
+        <v>-0.04909021779894829</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1219,7 +1219,7 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>-0.08345638960599899</v>
+        <v>0.01612738706171513</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1227,7 +1227,7 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>-0.104219451546669</v>
+        <v>-0.05210376530885696</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1235,7 +1235,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>0.03119462728500366</v>
+        <v>-0.05454245582222939</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1243,7 +1243,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>0.0153292790055275</v>
+        <v>-0.001893242471851408</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1251,7 +1251,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>-0.1115502417087555</v>
+        <v>-0.04166665300726891</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1259,7 +1259,7 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>-0.117349773645401</v>
+        <v>-0.03397499397397041</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1267,7 +1267,7 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>0.01186832971870899</v>
+        <v>-0.08233810216188431</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1275,7 +1275,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>-0.09243651479482651</v>
+        <v>-0.06814239174127579</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1283,7 +1283,7 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>0.01284540630877018</v>
+        <v>-0.01097240392118692</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1291,7 +1291,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>-0.04791238903999329</v>
+        <v>-0.05663706734776497</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1299,7 +1299,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>0.09776142984628677</v>
+        <v>-0.02505508065223694</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1307,7 +1307,7 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>-0.177085667848587</v>
+        <v>-0.0342939980328083</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1315,7 +1315,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>-0.1498364955186844</v>
+        <v>0.01235485635697842</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1323,7 +1323,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>-0.07098221033811569</v>
+        <v>-0.08740133792161942</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1331,7 +1331,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>-0.09102100878953934</v>
+        <v>0.005726086441427469</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1339,7 +1339,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>-0.1257243305444717</v>
+        <v>0.004742693156003952</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1347,7 +1347,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>0.0142872566357255</v>
+        <v>-0.05000568926334381</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1355,7 +1355,7 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>0.08417314291000366</v>
+        <v>0.01605942286550999</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1363,7 +1363,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>0.04573734849691391</v>
+        <v>0.04612843319773674</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1371,7 +1371,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>-0.06161119416356087</v>
+        <v>-0.0157275628298521</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1379,7 +1379,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>-0.07577408105134964</v>
+        <v>-0.06928671151399612</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1387,7 +1387,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>-0.02799687348306179</v>
+        <v>0.02476442791521549</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1395,7 +1395,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>-0.08818936347961426</v>
+        <v>-0.02782525680959225</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1403,7 +1403,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>-0.05357154831290245</v>
+        <v>0.02152431383728981</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1411,7 +1411,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>-0.05905858427286148</v>
+        <v>-0.006752686575055122</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1419,7 +1419,7 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>-0.08252659440040588</v>
+        <v>-0.0006433501257561147</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1427,7 +1427,7 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>-0.02610166370868683</v>
+        <v>-0.04508950933814049</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1435,7 +1435,7 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>-0.223819300532341</v>
+        <v>-0.02587642893195152</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1443,7 +1443,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>-0.01719782687723637</v>
+        <v>-0.0270231980830431</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1451,7 +1451,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>-0.1403121054172516</v>
+        <v>-0.006532173603773117</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1459,7 +1459,7 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>-0.09159887582063675</v>
+        <v>-0.05328363180160522</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1467,7 +1467,7 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>-0.01717574335634708</v>
+        <v>-0.09795290976762772</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1475,7 +1475,7 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>-0.01341797970235348</v>
+        <v>0.01896888576447964</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1483,7 +1483,7 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>0.1125528514385223</v>
+        <v>-0.04846331849694252</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1491,7 +1491,7 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>0.0160263404250145</v>
+        <v>-0.003385052317753434</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1499,7 +1499,7 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>-0.2157861143350601</v>
+        <v>-0.09989242255687714</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1507,7 +1507,7 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>-0.1157818287611008</v>
+        <v>-0.04493662342429161</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1515,7 +1515,7 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>0.01034658681601286</v>
+        <v>0.007204334251582623</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1523,7 +1523,7 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>0.02852902002632618</v>
+        <v>-0.01673361286520958</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1531,7 +1531,7 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>-0.07075043767690659</v>
+        <v>-0.06435196846723557</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1539,7 +1539,7 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>-0.109868049621582</v>
+        <v>-0.07080777734518051</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1547,7 +1547,7 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>-0.1217449530959129</v>
+        <v>-0.1142769902944565</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1555,7 +1555,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>-0.02578442916274071</v>
+        <v>0.01272721122950315</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1563,7 +1563,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>-0.1648226678371429</v>
+        <v>-0.01295905280858278</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1571,7 +1571,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>-0.09305427223443985</v>
+        <v>0.003281347453594208</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1579,7 +1579,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>0.03846374154090881</v>
+        <v>-0.05528610199689865</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1587,7 +1587,7 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>-0.04786640778183937</v>
+        <v>-0.07417339831590652</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1595,7 +1595,7 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>-0.03696935623884201</v>
+        <v>-0.007927651517093182</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1603,7 +1603,7 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>-0.01161142066121101</v>
+        <v>-0.08393402397632599</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1611,7 +1611,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>-0.2886662483215332</v>
+        <v>-0.0400700680911541</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1619,7 +1619,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>-0.02599031664431095</v>
+        <v>-0.02800003625452518</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1627,7 +1627,7 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>-0.1292381435632706</v>
+        <v>-0.0292271301150322</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1635,7 +1635,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>-0.09407097101211548</v>
+        <v>-0.06680292636156082</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1643,7 +1643,7 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>0.006170652341097593</v>
+        <v>-0.008409772999584675</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1651,7 +1651,7 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>-0.2061719000339508</v>
+        <v>-0.02932162210345268</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1659,7 +1659,7 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>-0.01436875853687525</v>
+        <v>-0.08703675866127014</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1667,7 +1667,7 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>-0.1053506731987</v>
+        <v>-0.09381962567567825</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1675,7 +1675,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>-0.07764020562171936</v>
+        <v>-0.06291677802801132</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1683,7 +1683,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>-0.04323693737387657</v>
+        <v>-0.005423332098871469</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1691,7 +1691,7 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>-0.008568167686462402</v>
+        <v>-0.01121558155864477</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1699,7 +1699,7 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>0.003309269901365042</v>
+        <v>-0.1518655121326447</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1707,7 +1707,7 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>0.007619281765073538</v>
+        <v>0.01616137847304344</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1715,7 +1715,7 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>-0.02671341225504875</v>
+        <v>0.01060223300009966</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1723,7 +1723,7 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>-0.09098653495311737</v>
+        <v>-0.02371115796267986</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1731,7 +1731,7 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>-0.1404056400060654</v>
+        <v>-0.03848818689584732</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1739,7 +1739,7 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>0.03424899280071259</v>
+        <v>0.04758840426802635</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1747,7 +1747,7 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>-0.03070328757166862</v>
+        <v>-0.05567159503698349</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1755,7 +1755,7 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>-0.06309251487255096</v>
+        <v>-0.07417029142379761</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1763,7 +1763,7 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>-0.1018646880984306</v>
+        <v>0.06408835202455521</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1771,7 +1771,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>-0.1801944822072983</v>
+        <v>-0.05075591802597046</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1779,7 +1779,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>-0.04336526989936829</v>
+        <v>-0.03937947750091553</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1787,7 +1787,7 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>-0.1643212139606476</v>
+        <v>-0.105917327105999</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1795,7 +1795,7 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>-0.1021283119916916</v>
+        <v>-0.03317529708147049</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1803,7 +1803,7 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>-0.2102445363998413</v>
+        <v>-0.03965567052364349</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1811,7 +1811,7 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>-0.04272372648119926</v>
+        <v>-0.09042225033044815</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1819,7 +1819,7 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>-0.1815572828054428</v>
+        <v>-0.04746860265731812</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1827,7 +1827,7 @@
         <v>129</v>
       </c>
       <c r="B131">
-        <v>-0.0637679323554039</v>
+        <v>-0.08238767087459564</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1835,7 +1835,7 @@
         <v>130</v>
       </c>
       <c r="B132">
-        <v>-0.1217350661754608</v>
+        <v>-0.04472554102540016</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1843,7 +1843,7 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>-0.0004472187429200858</v>
+        <v>0.006538607645779848</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1851,7 +1851,7 @@
         <v>132</v>
       </c>
       <c r="B134">
-        <v>-0.08752429485321045</v>
+        <v>-0.0894000455737114</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1859,7 +1859,7 @@
         <v>133</v>
       </c>
       <c r="B135">
-        <v>0.0124108549207449</v>
+        <v>-0.08560368418693542</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1867,7 +1867,7 @@
         <v>134</v>
       </c>
       <c r="B136">
-        <v>0.002325834473595023</v>
+        <v>0.04131008312106133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>